<commit_message>
file uploaded in Demo repository
</commit_message>
<xml_diff>
--- a/inputFiles/testData.xlsx
+++ b/inputFiles/testData.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="14190" windowHeight="5985" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="15705" windowHeight="5985"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -13,7 +13,7 @@
     <sheet name="Details" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="0"/>
-  <oleSize ref="A1:N17"/>
+  <oleSize ref="A1:O17"/>
 </workbook>
 </file>
 
@@ -393,8 +393,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:D4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -621,7 +621,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>

</xml_diff>